<commit_message>
add story lock to trigger story
</commit_message>
<xml_diff>
--- a/DataSource/excel/story.xlsx
+++ b/DataSource/excel/story.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21980" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20680" windowHeight="19760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="story.csv" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,24 @@
           </rPr>
           <t xml:space="preserve">
 15 show DialogSelections: selectionsId; selectionStoryId
-16 change logica data: logic Id;(parameter2 0:= , 1:add 2:minus 3:multiply 4:devide &gt;4: self-definition); value or expression; parameter4 = 0</t>
+16 change logica data: logic Id;(parameter2 0:= , 1:add 2:minus 3:multiply 4:devide &gt;4: self-definition</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>，-1：remove it</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>); value or expression; parameter4 = 0</t>
         </r>
         <r>
           <rPr>
@@ -137,6 +154,8 @@
           <t xml:space="preserve">表示3号为数值，1：表示3号为变量
 17 特殊的逻辑，例如 parameter1：表示功能如ship 表示添加船只,parameter2表示船只编号，parameter3表示船只名称，parameter4表示船舱货物
   paramter1 为npc的时候， parameter2 = 1表示入队， parameter2 = 3表示离队， parameter 3 为npcId
+18:决斗
+19 unlock/lock story, parameter1 0 unlock, 1 lock, parameter2 : storyId
 100：备注，不发生任何事情
 </t>
         </r>
@@ -185,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="211">
   <si>
     <t>storyId</t>
   </si>
@@ -812,6 +831,12 @@
   </si>
   <si>
     <t>Town_3.png</t>
+  </si>
+  <si>
+    <t>开启触发交易所剧情</t>
+  </si>
+  <si>
+    <t>交易品低价买入高价卖出，这是交易的基本常识。</t>
   </si>
 </sst>
 </file>
@@ -1901,11 +1926,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G217"/>
+  <dimension ref="A1:G219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D212" sqref="D212"/>
+      <pane ySplit="2" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D217" sqref="D217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5529,7 +5554,7 @@
       <c r="A158">
         <v>1</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="1" t="s">
         <v>147</v>
       </c>
       <c r="C158">
@@ -5552,7 +5577,7 @@
       <c r="A159">
         <v>1</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="1" t="s">
         <v>148</v>
       </c>
       <c r="C159">
@@ -5575,7 +5600,7 @@
       <c r="A160">
         <v>1</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="1" t="s">
         <v>149</v>
       </c>
       <c r="C160">
@@ -5598,7 +5623,7 @@
       <c r="A161">
         <v>1</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="1" t="s">
         <v>150</v>
       </c>
       <c r="C161">
@@ -5621,7 +5646,7 @@
       <c r="A162">
         <v>1</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B162" s="1" t="s">
         <v>151</v>
       </c>
       <c r="C162">
@@ -5644,7 +5669,7 @@
       <c r="A163">
         <v>1</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="1" t="s">
         <v>152</v>
       </c>
       <c r="C163">
@@ -5667,7 +5692,7 @@
       <c r="A164">
         <v>1</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B164" s="1" t="s">
         <v>153</v>
       </c>
       <c r="C164">
@@ -5690,7 +5715,7 @@
       <c r="A165">
         <v>1</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B165" s="1" t="s">
         <v>154</v>
       </c>
       <c r="C165">
@@ -5713,7 +5738,7 @@
       <c r="A166">
         <v>1</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C166">
@@ -5736,7 +5761,7 @@
       <c r="A167">
         <v>1</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B167" s="1" t="s">
         <v>156</v>
       </c>
       <c r="C167">
@@ -5759,7 +5784,7 @@
       <c r="A168">
         <v>1</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B168" s="1" t="s">
         <v>157</v>
       </c>
       <c r="C168">
@@ -5782,7 +5807,7 @@
       <c r="A169">
         <v>1</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B169" s="1" t="s">
         <v>158</v>
       </c>
       <c r="C169">
@@ -5805,7 +5830,7 @@
       <c r="A170">
         <v>1</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B170" s="1" t="s">
         <v>159</v>
       </c>
       <c r="C170">
@@ -5828,7 +5853,7 @@
       <c r="A171">
         <v>1</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="1" t="s">
         <v>160</v>
       </c>
       <c r="C171">
@@ -5851,7 +5876,7 @@
       <c r="A172">
         <v>1</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C172">
@@ -5874,7 +5899,7 @@
       <c r="A173">
         <v>1</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B173" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C173">
@@ -5897,7 +5922,7 @@
       <c r="A174">
         <v>1</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B174" s="1" t="s">
         <v>163</v>
       </c>
       <c r="C174">
@@ -5920,7 +5945,7 @@
       <c r="A175">
         <v>1</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B175" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C175">
@@ -5943,7 +5968,7 @@
       <c r="A176">
         <v>1</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B176" s="1" t="s">
         <v>165</v>
       </c>
       <c r="C176">
@@ -5966,7 +5991,7 @@
       <c r="A177">
         <v>1</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B177" s="1" t="s">
         <v>166</v>
       </c>
       <c r="C177">
@@ -5989,7 +6014,7 @@
       <c r="A178">
         <v>1</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B178" s="1" t="s">
         <v>167</v>
       </c>
       <c r="C178">
@@ -6012,7 +6037,7 @@
       <c r="A179">
         <v>1</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B179" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C179">
@@ -6035,7 +6060,7 @@
       <c r="A180">
         <v>1</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="1" t="s">
         <v>169</v>
       </c>
       <c r="C180">
@@ -6058,7 +6083,7 @@
       <c r="A181">
         <v>1</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B181" s="1" t="s">
         <v>170</v>
       </c>
       <c r="C181">
@@ -6081,7 +6106,7 @@
       <c r="A182">
         <v>1</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B182" s="1" t="s">
         <v>171</v>
       </c>
       <c r="C182">
@@ -6104,7 +6129,7 @@
       <c r="A183">
         <v>1</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B183" s="1" t="s">
         <v>172</v>
       </c>
       <c r="C183">
@@ -6127,7 +6152,7 @@
       <c r="A184">
         <v>1</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B184" s="1" t="s">
         <v>173</v>
       </c>
       <c r="C184">
@@ -6150,7 +6175,7 @@
       <c r="A185">
         <v>1</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B185" s="1" t="s">
         <v>174</v>
       </c>
       <c r="C185">
@@ -6173,7 +6198,7 @@
       <c r="A186">
         <v>1</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B186" s="1" t="s">
         <v>175</v>
       </c>
       <c r="C186">
@@ -6196,7 +6221,7 @@
       <c r="A187">
         <v>1</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B187" s="1" t="s">
         <v>176</v>
       </c>
       <c r="C187">
@@ -6219,7 +6244,7 @@
       <c r="A188">
         <v>1</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B188" s="1" t="s">
         <v>177</v>
       </c>
       <c r="C188">
@@ -6242,7 +6267,7 @@
       <c r="A189">
         <v>1</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B189" s="1" t="s">
         <v>178</v>
       </c>
       <c r="C189">
@@ -6265,7 +6290,7 @@
       <c r="A190">
         <v>1</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B190" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C190">
@@ -6288,7 +6313,7 @@
       <c r="A191">
         <v>1</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="1" t="s">
         <v>180</v>
       </c>
       <c r="C191">
@@ -6311,7 +6336,7 @@
       <c r="A192">
         <v>1</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B192" s="1" t="s">
         <v>181</v>
       </c>
       <c r="C192">
@@ -6334,7 +6359,7 @@
       <c r="A193">
         <v>1</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B193" s="1" t="s">
         <v>182</v>
       </c>
       <c r="C193">
@@ -6357,7 +6382,7 @@
       <c r="A194">
         <v>1</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B194" s="1" t="s">
         <v>183</v>
       </c>
       <c r="C194">
@@ -6380,7 +6405,7 @@
       <c r="A195">
         <v>1</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="1" t="s">
         <v>184</v>
       </c>
       <c r="C195">
@@ -6403,7 +6428,7 @@
       <c r="A196">
         <v>1</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B196" s="1" t="s">
         <v>185</v>
       </c>
       <c r="C196">
@@ -6426,7 +6451,7 @@
       <c r="A197">
         <v>1</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B197" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C197">
@@ -6449,7 +6474,7 @@
       <c r="A198">
         <v>1</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B198" s="1" t="s">
         <v>187</v>
       </c>
       <c r="C198">
@@ -6587,7 +6612,7 @@
       <c r="A204">
         <v>1</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B204" s="1" t="s">
         <v>190</v>
       </c>
       <c r="C204">
@@ -6610,7 +6635,7 @@
       <c r="A205">
         <v>1</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B205" s="1" t="s">
         <v>191</v>
       </c>
       <c r="C205">
@@ -6633,7 +6658,7 @@
       <c r="A206">
         <v>1</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B206" s="1" t="s">
         <v>192</v>
       </c>
       <c r="C206">
@@ -6656,7 +6681,7 @@
       <c r="A207">
         <v>1</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B207" s="1" t="s">
         <v>193</v>
       </c>
       <c r="C207">
@@ -6702,7 +6727,7 @@
       <c r="A209">
         <v>1</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B209" s="1" t="s">
         <v>194</v>
       </c>
       <c r="C209">
@@ -6794,7 +6819,7 @@
       <c r="A213">
         <v>1</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B213" s="1" t="s">
         <v>198</v>
       </c>
       <c r="C213">
@@ -6817,7 +6842,7 @@
       <c r="A214">
         <v>1</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B214" s="1" t="s">
         <v>199</v>
       </c>
       <c r="C214">
@@ -6863,7 +6888,7 @@
       <c r="A216">
         <v>1</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B216" s="1" t="s">
         <v>202</v>
       </c>
       <c r="C216">
@@ -6886,7 +6911,7 @@
       <c r="A217">
         <v>1</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B217" s="1" t="s">
         <v>203</v>
       </c>
       <c r="C217">
@@ -6902,6 +6927,52 @@
         <v>114</v>
       </c>
       <c r="G217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7">
+      <c r="A218">
+        <v>1</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C218">
+        <v>19</v>
+      </c>
+      <c r="D218">
+        <v>0</v>
+      </c>
+      <c r="E218">
+        <v>2</v>
+      </c>
+      <c r="F218">
+        <v>0</v>
+      </c>
+      <c r="G218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7">
+      <c r="A219">
+        <v>2</v>
+      </c>
+      <c r="B219" t="s">
+        <v>210</v>
+      </c>
+      <c r="C219">
+        <v>12</v>
+      </c>
+      <c r="D219">
+        <v>5</v>
+      </c>
+      <c r="E219">
+        <v>5</v>
+      </c>
+      <c r="F219">
+        <v>115</v>
+      </c>
+      <c r="G219">
         <v>0</v>
       </c>
     </row>

</xml_diff>